<commit_message>
Added more plotting functionality, and started with a better labeling system
</commit_message>
<xml_diff>
--- a/Labels/pretty_labels.xlsx
+++ b/Labels/pretty_labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pleun\Documents\Uni\CNS\Thesis\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pleun\Documents\Uni\CNS\Thesis\MScThesisCode\Labels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{D796684B-277E-47D8-8E20-B0C95C1CECC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A682ABF2-EFDD-466E-8506-FA44F7DDDAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={30CC18EF-0C0D-486C-80B5-BE4C307FBD46}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="341">
   <si>
     <t>Unknown</t>
   </si>
@@ -951,12 +951,6 @@
     <t>Right vertical ramus of the anterior segment of the lateral sulcus</t>
   </si>
   <si>
-    <t>of the lateral fissure</t>
-  </si>
-  <si>
-    <t>Suggestion</t>
-  </si>
-  <si>
     <t>Right posterior ramus of the lateral sulcus</t>
   </si>
   <si>
@@ -1057,13 +1051,40 @@
   </si>
   <si>
     <t>Right transverse temporal surcus</t>
+  </si>
+  <si>
+    <t>Lobe</t>
+  </si>
+  <si>
+    <t>Frontal</t>
+  </si>
+  <si>
+    <t>Occipipital</t>
+  </si>
+  <si>
+    <t>Parietal;Frontal</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>of the lateral fissure?</t>
+  </si>
+  <si>
+    <t>Goes over the central sulcus, which defines the boundary between the frontal and parietal lobe</t>
+  </si>
+  <si>
+    <t>Lower part of the central sulcus, which defines the boundary between the frontal and parietal lobe</t>
+  </si>
+  <si>
+    <t>Parietal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1078,12 +1099,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1443,21 +1458,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D166"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1468,10 +1484,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1481,8 +1500,11 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1492,8 +1514,11 @@
       <c r="C3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1503,8 +1528,11 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1514,8 +1542,14 @@
       <c r="C5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1525,8 +1559,14 @@
       <c r="C6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>335</v>
+      </c>
+      <c r="E6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1536,8 +1576,11 @@
       <c r="C7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1547,8 +1590,11 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1559,7 +1605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1569,8 +1615,11 @@
       <c r="C10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1581,7 +1630,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1592,7 +1641,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1603,7 +1652,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1614,7 +1663,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1625,7 +1674,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1812,7 +1861,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1823,7 +1872,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1834,7 +1883,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1845,7 +1894,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1856,7 +1905,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1867,7 +1916,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1878,7 +1927,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1889,7 +1938,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1900,7 +1949,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1910,11 +1959,11 @@
       <c r="C41" t="s">
         <v>205</v>
       </c>
-      <c r="D41" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1924,11 +1973,11 @@
       <c r="C42" t="s">
         <v>206</v>
       </c>
-      <c r="D42" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1938,11 +1987,11 @@
       <c r="C43" t="s">
         <v>207</v>
       </c>
-      <c r="D43" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1953,7 +2002,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1964,7 +2013,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1975,7 +2024,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1986,7 +2035,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2877,7 +2926,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
@@ -2888,7 +2937,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
@@ -2898,11 +2947,11 @@
       <c r="C130" t="s">
         <v>296</v>
       </c>
-      <c r="D130" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E130" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>129</v>
       </c>
@@ -2912,11 +2961,11 @@
       <c r="C131" t="s">
         <v>297</v>
       </c>
-      <c r="D131" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E131" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>130</v>
       </c>
@@ -2924,13 +2973,13 @@
         <v>154</v>
       </c>
       <c r="C132" t="s">
-        <v>300</v>
-      </c>
-      <c r="D132" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E132" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>131</v>
       </c>
@@ -2938,10 +2987,10 @@
         <v>155</v>
       </c>
       <c r="C133" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>132</v>
       </c>
@@ -2949,10 +2998,10 @@
         <v>156</v>
       </c>
       <c r="C134" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>133</v>
       </c>
@@ -2960,10 +3009,10 @@
         <v>157</v>
       </c>
       <c r="C135" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>134</v>
       </c>
@@ -2971,10 +3020,10 @@
         <v>158</v>
       </c>
       <c r="C136" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>135</v>
       </c>
@@ -2982,10 +3031,10 @@
         <v>159</v>
       </c>
       <c r="C137" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>136</v>
       </c>
@@ -2993,10 +3042,10 @@
         <v>160</v>
       </c>
       <c r="C138" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>137</v>
       </c>
@@ -3004,10 +3053,10 @@
         <v>161</v>
       </c>
       <c r="C139" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>138</v>
       </c>
@@ -3015,10 +3064,10 @@
         <v>162</v>
       </c>
       <c r="C140" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139</v>
       </c>
@@ -3026,10 +3075,10 @@
         <v>163</v>
       </c>
       <c r="C141" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>140</v>
       </c>
@@ -3037,10 +3086,10 @@
         <v>164</v>
       </c>
       <c r="C142" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>141</v>
       </c>
@@ -3048,10 +3097,10 @@
         <v>165</v>
       </c>
       <c r="C143" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>142</v>
       </c>
@@ -3059,7 +3108,7 @@
         <v>166</v>
       </c>
       <c r="C144" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -3070,7 +3119,7 @@
         <v>167</v>
       </c>
       <c r="C145" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -3081,7 +3130,7 @@
         <v>168</v>
       </c>
       <c r="C146" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -3092,7 +3141,7 @@
         <v>169</v>
       </c>
       <c r="C147" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -3103,7 +3152,7 @@
         <v>170</v>
       </c>
       <c r="C148" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -3114,7 +3163,7 @@
         <v>171</v>
       </c>
       <c r="C149" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -3125,7 +3174,7 @@
         <v>172</v>
       </c>
       <c r="C150" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -3136,7 +3185,7 @@
         <v>173</v>
       </c>
       <c r="C151" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -3147,7 +3196,7 @@
         <v>174</v>
       </c>
       <c r="C152" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -3158,7 +3207,7 @@
         <v>175</v>
       </c>
       <c r="C153" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -3169,7 +3218,7 @@
         <v>176</v>
       </c>
       <c r="C154" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -3180,7 +3229,7 @@
         <v>177</v>
       </c>
       <c r="C155" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -3191,7 +3240,7 @@
         <v>178</v>
       </c>
       <c r="C156" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -3202,7 +3251,7 @@
         <v>179</v>
       </c>
       <c r="C157" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -3213,7 +3262,7 @@
         <v>180</v>
       </c>
       <c r="C158" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
@@ -3224,7 +3273,7 @@
         <v>181</v>
       </c>
       <c r="C159" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -3235,7 +3284,7 @@
         <v>182</v>
       </c>
       <c r="C160" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -3246,7 +3295,7 @@
         <v>183</v>
       </c>
       <c r="C161" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -3257,7 +3306,7 @@
         <v>184</v>
       </c>
       <c r="C162" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -3268,7 +3317,7 @@
         <v>185</v>
       </c>
       <c r="C163" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -3279,7 +3328,7 @@
         <v>186</v>
       </c>
       <c r="C164" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -3290,7 +3339,7 @@
         <v>187</v>
       </c>
       <c r="C165" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added new functions and updated functions wow what a commit message
</commit_message>
<xml_diff>
--- a/Labels/pretty_labels.xlsx
+++ b/Labels/pretty_labels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pleun\Documents\Uni\CNS\Thesis\MScThesisCode\Labels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A682ABF2-EFDD-466E-8506-FA44F7DDDAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50DA8CA-C8CB-4FD1-B525-2755C9967616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="351">
   <si>
     <t>Unknown</t>
   </si>
@@ -1059,12 +1059,6 @@
     <t>Frontal</t>
   </si>
   <si>
-    <t>Occipipital</t>
-  </si>
-  <si>
-    <t>Parietal;Frontal</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -1078,13 +1072,49 @@
   </si>
   <si>
     <t>Parietal</t>
+  </si>
+  <si>
+    <t>Limbic</t>
+  </si>
+  <si>
+    <t>Occipital</t>
+  </si>
+  <si>
+    <t>Occipital;Temporal</t>
+  </si>
+  <si>
+    <t>Temporal</t>
+  </si>
+  <si>
+    <t>of the lateral fissure? Both is possible</t>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/articles/10.3389/fnana.2018.00093/full</t>
+  </si>
+  <si>
+    <t>Occipital;Parietal</t>
+  </si>
+  <si>
+    <t>Frontal;Parietal</t>
+  </si>
+  <si>
+    <t>Limbic;Parietal</t>
+  </si>
+  <si>
+    <t>Subcortical</t>
+  </si>
+  <si>
+    <t>Insular</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1096,6 +1126,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1118,14 +1156,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1462,7 +1503,7 @@
   <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1487,7 +1528,7 @@
         <v>332</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1529,7 +1570,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1543,10 +1584,10 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="E5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1560,10 +1601,10 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="E6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1604,6 +1645,9 @@
       <c r="C9" t="s">
         <v>33</v>
       </c>
+      <c r="D9" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1616,7 +1660,7 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1629,6 +1673,9 @@
       <c r="C11" t="s">
         <v>35</v>
       </c>
+      <c r="D11" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1640,6 +1687,9 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
+      <c r="D12" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1651,6 +1701,9 @@
       <c r="C13" t="s">
         <v>37</v>
       </c>
+      <c r="D13" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1662,6 +1715,9 @@
       <c r="C14" t="s">
         <v>38</v>
       </c>
+      <c r="D14" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1673,6 +1729,9 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
+      <c r="D15" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1684,8 +1743,11 @@
       <c r="C16" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1695,8 +1757,11 @@
       <c r="C17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1706,8 +1771,11 @@
       <c r="C18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1717,8 +1785,11 @@
       <c r="C19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1728,8 +1799,11 @@
       <c r="C20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1739,8 +1813,11 @@
       <c r="C21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1750,8 +1827,11 @@
       <c r="C22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1761,8 +1841,11 @@
       <c r="C23" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1772,8 +1855,11 @@
       <c r="C24" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1783,8 +1869,11 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1794,8 +1883,11 @@
       <c r="C26" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1805,8 +1897,11 @@
       <c r="C27" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1816,8 +1911,11 @@
       <c r="C28" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1827,8 +1925,11 @@
       <c r="C29" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1838,8 +1939,11 @@
       <c r="C30" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1849,8 +1953,11 @@
       <c r="C31" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1859,6 +1966,9 @@
       </c>
       <c r="C32" t="s">
         <v>195</v>
+      </c>
+      <c r="D32" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1871,6 +1981,9 @@
       <c r="C33" t="s">
         <v>196</v>
       </c>
+      <c r="D33" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -1882,6 +1995,9 @@
       <c r="C34" t="s">
         <v>197</v>
       </c>
+      <c r="D34" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -1893,6 +2009,9 @@
       <c r="C35" t="s">
         <v>198</v>
       </c>
+      <c r="D35" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -1904,6 +2023,9 @@
       <c r="C36" t="s">
         <v>199</v>
       </c>
+      <c r="D36" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -1915,6 +2037,9 @@
       <c r="C37" t="s">
         <v>200</v>
       </c>
+      <c r="D37" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -1926,6 +2051,9 @@
       <c r="C38" t="s">
         <v>201</v>
       </c>
+      <c r="D38" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
@@ -1937,6 +2065,9 @@
       <c r="C39" t="s">
         <v>202</v>
       </c>
+      <c r="D39" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -1948,6 +2079,9 @@
       <c r="C40" t="s">
         <v>203</v>
       </c>
+      <c r="D40" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -1959,8 +2093,11 @@
       <c r="C41" t="s">
         <v>205</v>
       </c>
+      <c r="D41" t="s">
+        <v>342</v>
+      </c>
       <c r="E41" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1973,8 +2110,11 @@
       <c r="C42" t="s">
         <v>206</v>
       </c>
+      <c r="D42" t="s">
+        <v>342</v>
+      </c>
       <c r="E42" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1987,8 +2127,11 @@
       <c r="C43" t="s">
         <v>207</v>
       </c>
+      <c r="D43" t="s">
+        <v>342</v>
+      </c>
       <c r="E43" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2001,6 +2144,9 @@
       <c r="C44" t="s">
         <v>208</v>
       </c>
+      <c r="D44" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -2012,6 +2158,9 @@
       <c r="C45" t="s">
         <v>209</v>
       </c>
+      <c r="D45" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -2023,6 +2172,9 @@
       <c r="C46" t="s">
         <v>210</v>
       </c>
+      <c r="D46" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -2034,6 +2186,9 @@
       <c r="C47" t="s">
         <v>211</v>
       </c>
+      <c r="D47" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -2045,8 +2200,11 @@
       <c r="C48" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2056,8 +2214,11 @@
       <c r="C49" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2067,8 +2228,11 @@
       <c r="C50" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2078,8 +2242,11 @@
       <c r="C51" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2089,8 +2256,11 @@
       <c r="C52" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2100,8 +2270,11 @@
       <c r="C53" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2111,8 +2284,11 @@
       <c r="C54" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2122,8 +2298,11 @@
       <c r="C55" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2133,8 +2312,11 @@
       <c r="C56" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2144,8 +2326,14 @@
       <c r="C57" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>338</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2155,8 +2343,11 @@
       <c r="C58" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2166,8 +2357,11 @@
       <c r="C59" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2177,8 +2371,11 @@
       <c r="C60" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2188,8 +2385,11 @@
       <c r="C61" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2199,8 +2399,11 @@
       <c r="C62" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2210,8 +2413,11 @@
       <c r="C63" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2221,8 +2427,11 @@
       <c r="C64" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2232,8 +2441,11 @@
       <c r="C65" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2243,8 +2455,11 @@
       <c r="C66" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2254,8 +2469,11 @@
       <c r="C67" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2265,8 +2483,11 @@
       <c r="C68" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2276,8 +2497,11 @@
       <c r="C69" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2287,8 +2511,11 @@
       <c r="C70" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -2298,8 +2525,11 @@
       <c r="C71" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2309,8 +2539,11 @@
       <c r="C72" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2320,8 +2553,11 @@
       <c r="C73" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2331,8 +2567,11 @@
       <c r="C74" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -2342,8 +2581,11 @@
       <c r="C75" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2353,8 +2595,11 @@
       <c r="C76" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2364,8 +2609,11 @@
       <c r="C77" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2375,8 +2623,11 @@
       <c r="C78" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -2386,8 +2637,11 @@
       <c r="C79" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -2397,8 +2651,11 @@
       <c r="C80" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -2408,8 +2665,11 @@
       <c r="C81" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -2419,8 +2679,14 @@
       <c r="C82" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>342</v>
+      </c>
+      <c r="E82" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2430,8 +2696,11 @@
       <c r="C83" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2441,8 +2710,11 @@
       <c r="C84" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2452,8 +2724,11 @@
       <c r="C85" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2463,8 +2738,11 @@
       <c r="C86" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2474,8 +2752,11 @@
       <c r="C87" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2485,8 +2766,11 @@
       <c r="C88" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2496,8 +2780,11 @@
       <c r="C89" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2507,8 +2794,11 @@
       <c r="C90" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -2518,8 +2808,11 @@
       <c r="C91" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2529,8 +2822,11 @@
       <c r="C92" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2540,8 +2836,11 @@
       <c r="C93" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2551,8 +2850,11 @@
       <c r="C94" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2562,8 +2864,11 @@
       <c r="C95" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2573,8 +2878,11 @@
       <c r="C96" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -2584,8 +2892,11 @@
       <c r="C97" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -2595,8 +2906,11 @@
       <c r="C98" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -2606,8 +2920,11 @@
       <c r="C99" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2617,8 +2934,11 @@
       <c r="C100" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -2628,8 +2948,11 @@
       <c r="C101" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -2639,8 +2962,11 @@
       <c r="C102" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
@@ -2650,8 +2976,11 @@
       <c r="C103" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
@@ -2661,8 +2990,11 @@
       <c r="C104" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
@@ -2672,8 +3004,11 @@
       <c r="C105" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -2683,8 +3018,11 @@
       <c r="C106" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
@@ -2694,8 +3032,11 @@
       <c r="C107" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
@@ -2705,8 +3046,11 @@
       <c r="C108" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
@@ -2716,8 +3060,11 @@
       <c r="C109" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
@@ -2727,8 +3074,11 @@
       <c r="C110" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
@@ -2738,8 +3088,11 @@
       <c r="C111" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
@@ -2749,8 +3102,11 @@
       <c r="C112" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
@@ -2760,8 +3116,11 @@
       <c r="C113" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
@@ -2771,8 +3130,11 @@
       <c r="C114" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
@@ -2782,8 +3144,11 @@
       <c r="C115" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
@@ -2793,8 +3158,11 @@
       <c r="C116" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
@@ -2804,8 +3172,11 @@
       <c r="C117" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
@@ -2815,8 +3186,11 @@
       <c r="C118" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
@@ -2826,8 +3200,11 @@
       <c r="C119" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
@@ -2837,8 +3214,11 @@
       <c r="C120" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
@@ -2848,8 +3228,11 @@
       <c r="C121" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
@@ -2859,8 +3242,11 @@
       <c r="C122" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
@@ -2870,8 +3256,11 @@
       <c r="C123" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
@@ -2881,8 +3270,11 @@
       <c r="C124" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
@@ -2892,8 +3284,11 @@
       <c r="C125" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
@@ -2903,8 +3298,11 @@
       <c r="C126" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
@@ -2914,8 +3312,11 @@
       <c r="C127" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
@@ -2924,6 +3325,9 @@
       </c>
       <c r="C128" t="s">
         <v>294</v>
+      </c>
+      <c r="D128" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2936,6 +3340,9 @@
       <c r="C129" t="s">
         <v>295</v>
       </c>
+      <c r="D129" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
@@ -2947,8 +3354,11 @@
       <c r="C130" t="s">
         <v>296</v>
       </c>
+      <c r="D130" t="s">
+        <v>342</v>
+      </c>
       <c r="E130" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2961,8 +3371,11 @@
       <c r="C131" t="s">
         <v>297</v>
       </c>
+      <c r="D131" t="s">
+        <v>342</v>
+      </c>
       <c r="E131" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2975,8 +3388,11 @@
       <c r="C132" t="s">
         <v>298</v>
       </c>
+      <c r="D132" t="s">
+        <v>342</v>
+      </c>
       <c r="E132" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -2989,6 +3405,9 @@
       <c r="C133" t="s">
         <v>299</v>
       </c>
+      <c r="D133" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
@@ -3000,6 +3419,9 @@
       <c r="C134" t="s">
         <v>300</v>
       </c>
+      <c r="D134" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
@@ -3011,6 +3433,9 @@
       <c r="C135" t="s">
         <v>301</v>
       </c>
+      <c r="D135" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
@@ -3022,6 +3447,9 @@
       <c r="C136" t="s">
         <v>302</v>
       </c>
+      <c r="D136" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
@@ -3033,6 +3461,9 @@
       <c r="C137" t="s">
         <v>303</v>
       </c>
+      <c r="D137" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
@@ -3044,6 +3475,9 @@
       <c r="C138" t="s">
         <v>304</v>
       </c>
+      <c r="D138" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
@@ -3055,6 +3489,9 @@
       <c r="C139" t="s">
         <v>305</v>
       </c>
+      <c r="D139" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
@@ -3066,6 +3503,9 @@
       <c r="C140" t="s">
         <v>306</v>
       </c>
+      <c r="D140" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
@@ -3077,6 +3517,9 @@
       <c r="C141" t="s">
         <v>307</v>
       </c>
+      <c r="D141" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
@@ -3088,6 +3531,9 @@
       <c r="C142" t="s">
         <v>308</v>
       </c>
+      <c r="D142" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
@@ -3099,6 +3545,9 @@
       <c r="C143" t="s">
         <v>309</v>
       </c>
+      <c r="D143" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
@@ -3110,8 +3559,11 @@
       <c r="C144" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>143</v>
       </c>
@@ -3121,8 +3573,11 @@
       <c r="C145" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D145" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>144</v>
       </c>
@@ -3132,8 +3587,11 @@
       <c r="C146" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D146" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>145</v>
       </c>
@@ -3143,8 +3601,11 @@
       <c r="C147" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D147" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>146</v>
       </c>
@@ -3154,8 +3615,11 @@
       <c r="C148" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D148" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>147</v>
       </c>
@@ -3165,8 +3629,11 @@
       <c r="C149" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>148</v>
       </c>
@@ -3176,8 +3643,11 @@
       <c r="C150" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>149</v>
       </c>
@@ -3187,8 +3657,11 @@
       <c r="C151" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D151" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>150</v>
       </c>
@@ -3198,8 +3671,11 @@
       <c r="C152" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D152" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>151</v>
       </c>
@@ -3209,8 +3685,11 @@
       <c r="C153" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D153" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>152</v>
       </c>
@@ -3220,8 +3699,11 @@
       <c r="C154" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D154" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>153</v>
       </c>
@@ -3231,8 +3713,11 @@
       <c r="C155" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D155" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>154</v>
       </c>
@@ -3242,8 +3727,11 @@
       <c r="C156" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D156" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>155</v>
       </c>
@@ -3253,8 +3741,11 @@
       <c r="C157" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D157" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>156</v>
       </c>
@@ -3264,8 +3755,11 @@
       <c r="C158" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D158" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>157</v>
       </c>
@@ -3275,8 +3769,11 @@
       <c r="C159" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D159" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>158</v>
       </c>
@@ -3286,8 +3783,11 @@
       <c r="C160" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D160" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>159</v>
       </c>
@@ -3297,8 +3797,11 @@
       <c r="C161" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D161" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>160</v>
       </c>
@@ -3308,8 +3811,11 @@
       <c r="C162" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D162" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>161</v>
       </c>
@@ -3319,8 +3825,11 @@
       <c r="C163" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D163" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>162</v>
       </c>
@@ -3330,8 +3839,11 @@
       <c r="C164" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D164" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>163</v>
       </c>
@@ -3341,8 +3853,11 @@
       <c r="C165" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D165" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>164</v>
       </c>
@@ -3352,10 +3867,16 @@
       <c r="C166" t="s">
         <v>256</v>
       </c>
+      <c r="D166" t="s">
+        <v>348</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E57" r:id="rId1" xr:uid="{4F3A2A06-F909-4405-BC8E-8F5EF70EA20D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>